<commit_message>
add round up 4 decimals
</commit_message>
<xml_diff>
--- a/data-set/i-0677593b0a3baf02b.xlsx
+++ b/data-set/i-0677593b0a3baf02b.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1750,6 +1750,342 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>12:15:28</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2.2923497267759094</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>3527.2</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>3081.6</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>42.8</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>42.8</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>12:22:40</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>3434.0</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>3087.4</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>43.8</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>43.2</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>12:23:18</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>3416.0</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>3052.2</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>43.8</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>43.2</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>12:24:08</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2.3003</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>3466.8</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>3077.8</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>43.8</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>43.2</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>12:24:39</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2.3002593312956856</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>3466.8</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>3077.8</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>43.8</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>43.2</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>12:25:00</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2.3079</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>3424.0</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>3045.6</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>42.4</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>42.6</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>12:25:13</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2.3079</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>3424.0</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>3045.6</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>42.4</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>42.6</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>12:27:28</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2.2667</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>3406.0</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>3030.4</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>42.4</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>42.6</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
change datatime to be utc
</commit_message>
<xml_diff>
--- a/data-set/i-0677593b0a3baf02b.xlsx
+++ b/data-set/i-0677593b0a3baf02b.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2086,6 +2086,1089 @@
         </is>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>12:33:11</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2.233</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>4598.6</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>5254.4</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>50.2</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>51.6</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>12:38:29</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2.5333</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>4491.4</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>6011.6</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>51.2</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>51.2</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>12:38:57</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2.5333</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>4491.4</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>6011.6</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>51.2</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>51.2</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>12:41:16</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2.5333</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>4196.2</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>5886.8</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>43.0</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>43.4</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>12:41:32</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2.3333</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>12:41:49</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2.3333</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>15:43:04</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>15:44:15</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>16:28:34</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>16:33:13</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>4.8333</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2990.0</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2964.0</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>16:33:38</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>4.8333</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2990.0</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2964.0</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>16:37:00</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>6634.0</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>7839.0</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>16:40:07</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>2.3333</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>3392.0</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2952.0</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>16:41:04</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>2.2951</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>16:42:25</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>2.3729</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>3426.0</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>16:43:24</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>20.8333</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>5399.0</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>3644.0</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>16:43:49</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>20.8333</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>5399.0</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>3644.0</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>16:44:56</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>25.1667</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>5764.0</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>5536.0</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>16:45:56</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>27.3333</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>6965.0</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>5536.0</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>16:47:05</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>29.5</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>7989.0</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>6688.0</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>16:48:18</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>6.0656</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>4828.0</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>5196.0</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>16:49:24</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2536.0</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>2444.0</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>16:50:24</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2674.0</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>2312.0</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>16:51:24</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2682.0</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>2548.0</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>16:52:24</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>4950.0</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>4937.0</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>16:53:24</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>2.3333</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>3450.0</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>3176.0</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>16:57:55</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>2.7869</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>3930.0</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>3948.0</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>16:59:02</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>2.2951</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>5751.0</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>5739.0</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>17:00:02</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>21.3115</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>5695.0</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>3984.0</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>17:01:02</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>31.5517</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>8878.0</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>7791.0</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>17:02:02</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>29.0323</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>7023.0</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>5476.0</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>12.931</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>5137.0</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>4804.0</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>17:04:02</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>20.8197</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>11172.0</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>10636.0</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>17:05:02</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>21.3333</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>6219.0</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>5836.0</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
create autoscaling file and rename the app
</commit_message>
<xml_diff>
--- a/data-set/i-0677593b0a3baf02b.xlsx
+++ b/data-set/i-0677593b0a3baf02b.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3169,6 +3169,582 @@
         </is>
       </c>
     </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>17:38:49</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>2.3333</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>3336.0</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>2924.0</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>17:40:34</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>2.3729</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>5391.0</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>5733.0</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>17:41:41</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>2.2951</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>5792.0</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>5661.0</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>17:42:41</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>3.5593</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>14308.0</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>12436.0</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>17:43:41</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>2.623</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>6926.0</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>5312.0</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>17:44:41</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>2.8333</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>5812.0</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>4232.0</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>17:45:41</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>2.8333</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>7288.0</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>5856.0</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>17:46:41</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>2.8333</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>7810.0</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>6112.0</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>17:47:41</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>0.8333</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>5318.0</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>3500.0</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>17:48:41</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>9102.0</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>7301.0</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>17:49:41</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>2.623</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>5688.0</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>4540.0</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>17:50:41</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>1.8644</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>6976.0</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>5144.0</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>17:51:41</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>3.8333</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>6176.0</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>4541.0</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>17:52:41</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>2.6667</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>5708.0</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>4332.0</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>17:53:41</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>2.3333</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>9732.0</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>7712.0</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>18:19:24</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>2.3333</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>3550.0</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>3064.0</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>18:19:57</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>2.2951</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>5511.0</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>5870.0</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>18:20:12</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>2.2951</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>5511.0</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>5870.0</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>